<commit_message>
Manifest data Upload page work
</commit_message>
<xml_diff>
--- a/src/assets/static-content/Passengers.xlsx
+++ b/src/assets/static-content/Passengers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PAL_CMS_Git_03052017\ERSClient\src\assets\static-content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PAL_CMS_GIT_CODE_ITERATION2\ERSClient-Iteration2\src\assets\static-content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Passenger's Name</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Passenger's Nationality</t>
-  </si>
-  <si>
-    <t>Affected Flight Number</t>
   </si>
   <si>
     <t>Baggage Weight(In KG)</t>
@@ -408,93 +405,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>